<commit_message>
added product code to SD-Connect
</commit_message>
<xml_diff>
--- a/scripts/reports/gsp_transport/resource/mapping_table.xlsx
+++ b/scripts/reports/gsp_transport/resource/mapping_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1319639\Development\orion_report_management_tool\scripts\reports\gsp_transport\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB6F58E-CECC-4898-BBCF-0540834D4460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FC14BB-1D34-41EC-83F7-2189BF33BE75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45" yWindow="-18135" windowWidth="29070" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,13 +807,20 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,20 +831,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -847,19 +858,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1218,7 +1218,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1264,180 +1264,180 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="29" t="s">
+      <c r="G2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="30" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="29" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="30" t="s">
+      <c r="D4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="29" t="s">
+      <c r="G4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="30" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="29" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="29" t="s">
+      <c r="G6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="29" t="s">
+      <c r="I6" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
       <c r="E7" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="30" t="s">
+      <c r="D8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="30" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="31"/>
+      <c r="G9" s="16"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="31"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="29" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="29" t="s">
+      <c r="D10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1446,161 +1446,161 @@
       <c r="F10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="29" t="s">
+      <c r="I10" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
       <c r="E11" s="7" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="16"/>
       <c r="H11" s="20"/>
-      <c r="I11" s="31"/>
+      <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="29" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="30" t="s">
+      <c r="D12" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="29" t="s">
+      <c r="I12" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="30" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="12" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="31"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="20"/>
-      <c r="I13" s="31"/>
+      <c r="I13" s="16"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="21" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="30" t="s">
+      <c r="D14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="15"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="29"/>
+      <c r="I14" s="15"/>
     </row>
     <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="28"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="30" t="s">
+      <c r="A15" s="22"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="31"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="1:9" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="28"/>
-      <c r="C16" s="30" t="s">
+      <c r="A16" s="22"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="12" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="30" t="s">
+      <c r="C18" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="30" t="s">
+      <c r="D18" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="12" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="7" t="s">
@@ -1612,33 +1612,33 @@
       <c r="H18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="33" t="s">
+      <c r="A19" s="17"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="30" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="12" t="s">
         <v>24</v>
       </c>
       <c r="F20" s="7" t="s">
@@ -1650,184 +1650,153 @@
       <c r="H20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I20" s="30" t="s">
+      <c r="I20" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I21" s="35" t="s">
+      <c r="I21" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="12"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35" t="s">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="35" t="s">
+      <c r="G22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I22" s="35" t="s">
+      <c r="I22" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="14" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G23" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="35" t="s">
+      <c r="I23" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35" t="s">
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="12"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="35" t="s">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="35" t="s">
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="I25" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="12"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="35" t="s">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="35" t="s">
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="35" t="s">
+      <c r="I26" s="14" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="47">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
@@ -1844,6 +1813,37 @@
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1855,7 +1855,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -1902,16 +1902,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -1920,38 +1920,38 @@
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="13" t="s">
+      <c r="G2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
       <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="28"/>
-      <c r="C4" s="21" t="s">
+      <c r="A4" s="22"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -1960,38 +1960,38 @@
       <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="28"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
       <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="21" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -2000,42 +2000,42 @@
       <c r="F6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="G6" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="28" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="18"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
       <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
       <c r="I7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2044,38 +2044,38 @@
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="28" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="29"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="14"/>
+      <c r="I9" s="29"/>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="21" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -2084,7 +2084,7 @@
       <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="19" t="s">
@@ -2093,29 +2093,29 @@
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
       <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="29"/>
       <c r="H11" s="20"/>
       <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="21" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="30" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -2124,7 +2124,7 @@
       <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="G12" s="28" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="19" t="s">
@@ -2133,30 +2133,30 @@
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="14"/>
+      <c r="G13" s="29"/>
       <c r="H13" s="20"/>
       <c r="I13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="28" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2165,31 +2165,31 @@
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="19"/>
-      <c r="I14" s="13"/>
+      <c r="I14" s="28"/>
     </row>
     <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="17"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="14"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="14"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="29"/>
       <c r="H15" s="20"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:9" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="22"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2207,8 +2207,8 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="18"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2226,10 +2226,10 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="17" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2255,8 +2255,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
@@ -2268,8 +2268,8 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2295,30 +2295,6 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="38">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="G8:G9"/>
@@ -2333,6 +2309,30 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
support CEVN and SD-Connect services
</commit_message>
<xml_diff>
--- a/scripts/reports/gsp_transport/resource/mapping_table.xlsx
+++ b/scripts/reports/gsp_transport/resource/mapping_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p1319639\Development\orion_report_management_tool\scripts\reports\gsp_transport\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E913AE0C-1D31-48F8-9330-4EAD024721D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FC85B9-CECF-467F-993B-793A79D890BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-18135" windowWidth="29070" windowHeight="17670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28845" yWindow="-16470" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="20231214" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="57">
   <si>
     <t>Service</t>
   </si>
@@ -180,9 +180,6 @@
 ELK0003</t>
   </si>
   <si>
-    <t>GDST Co-ordination Work</t>
-  </si>
-  <si>
     <t>CEVN</t>
   </si>
   <si>
@@ -229,10 +226,13 @@
     <t>Check COM Date</t>
   </si>
   <si>
-    <t>Yes, if Co-ordination queue is not COM and customer is SINGNET</t>
-  </si>
-  <si>
     <t>Yes, and copy to Co-ordination columns</t>
+  </si>
+  <si>
+    <t>GSDT Co-ordination Work</t>
+  </si>
+  <si>
+    <t>Yes, if customer is SINGNET</t>
   </si>
 </sst>
 </file>
@@ -992,18 +992,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1051,7 +1049,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1072,10 +1070,213 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1084,218 +1285,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1653,10 +1660,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961FAA7C-FAC3-4FE3-83F1-C557563741C6}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1666,534 +1674,497 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.44140625" customWidth="1"/>
+    <col min="6" max="6" width="37.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="60" t="s">
+      <c r="E1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="60" t="s">
+      <c r="F1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="61"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="63"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="61"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="61"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="63"/>
+    </row>
+    <row r="6" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="61"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="36"/>
+      <c r="E6" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="62"/>
+      <c r="B7" s="54"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="48"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="56"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="36"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="63"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="56"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="59" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="36"/>
+      <c r="E10" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="36"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="56"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="36"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="63"/>
+    </row>
+    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="56"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="36"/>
+      <c r="E12" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="36"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="72" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="57"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="31"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="48"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="61" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="62" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="63" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="64" t="s">
+      <c r="G14" s="49"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="46"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="61"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="58"/>
+      <c r="D15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="36"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="47"/>
+    </row>
+    <row r="16" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="61"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="36"/>
+      <c r="G16" s="50"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="47"/>
+    </row>
+    <row r="17" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="62"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="31"/>
+      <c r="E17" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="31"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="48"/>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="65" t="s">
+      <c r="D18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="66" t="s">
+      <c r="F18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="65" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="67" t="s">
+      <c r="G18" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="I18" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="35" t="s">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="56"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="18"/>
+    </row>
+    <row r="20" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="92"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="90" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="90" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="90" t="s">
+        <v>33</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="73" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="93" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="48"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="47"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="31" t="s">
+      <c r="I21" s="43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="65"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="46" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="91" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="44"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="66"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="45"/>
+    </row>
+    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="70" t="s">
+        <v>52</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="H24" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="I24" s="44" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="47"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="48"/>
-    </row>
-    <row r="6" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="31" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="65"/>
+      <c r="B25" s="70"/>
+      <c r="C25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="44"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="66"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="29"/>
-      <c r="E6" s="41" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="68"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="70"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="74"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="65" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="66" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="65" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="76" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="67" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="29"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="48"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="29"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="48"/>
-    </row>
-    <row r="12" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G12" s="29"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="77"/>
-      <c r="B13" s="70"/>
-      <c r="C13" s="70"/>
-      <c r="D13" s="71"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="73" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="71"/>
-      <c r="H13" s="72"/>
-      <c r="I13" s="74"/>
-    </row>
-    <row r="14" spans="1:9" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="67"/>
-    </row>
-    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="47"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="50"/>
-    </row>
-    <row r="16" spans="1:9" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="47"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="32" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="29"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="50"/>
-    </row>
-    <row r="17" spans="1:9" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="68"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="71"/>
-      <c r="E17" s="73" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="71"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="74"/>
-    </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="64" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="66" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="66" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="66" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="H18" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="82" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="51"/>
-    </row>
-    <row r="20" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="77"/>
-      <c r="B20" s="70"/>
-      <c r="C20" s="78" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="78" t="s">
-        <v>24</v>
-      </c>
-      <c r="F20" s="73" t="s">
-        <v>26</v>
-      </c>
-      <c r="G20" s="73" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="I20" s="83" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="84" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="85" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="86" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="87" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="87" t="s">
-        <v>42</v>
-      </c>
-      <c r="H21" s="87" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="89" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="52"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="53"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="54"/>
-      <c r="B23" s="90"/>
-      <c r="C23" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="91"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="57"/>
-      <c r="I23" s="58"/>
-    </row>
-    <row r="24" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="79" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="80" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="44" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" s="53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="52"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="53"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="54"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="56" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="58"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="45"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="53">
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="G21:G23"/>
-    <mergeCell ref="G24:G26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="F24:F26"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="H8:H13"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="I14:I17"/>
-    <mergeCell ref="G14:G17"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="F14:F17"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D7"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D8:D13"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="B24:B26"/>
@@ -2208,6 +2179,45 @@
     <mergeCell ref="A14:A17"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C14:C15"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="G2:G7"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D7"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="G14:G17"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="F14:F17"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="I24:I26"/>
+    <mergeCell ref="I14:I17"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="G21:G23"/>
+    <mergeCell ref="G24:G26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2266,16 +2276,16 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="8" t="s">
@@ -2284,38 +2294,38 @@
       <c r="F2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="21" t="s">
+      <c r="G2" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="74" t="s">
         <v>10</v>
       </c>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="85"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="78"/>
+      <c r="D3" s="78"/>
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
       <c r="I3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="19" t="s">
+      <c r="A4" s="85"/>
+      <c r="B4" s="87"/>
+      <c r="C4" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="8" t="s">
@@ -2324,38 +2334,38 @@
       <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="21" t="s">
+      <c r="G4" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="74" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="85"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
       <c r="E5" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
       <c r="I5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="85"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -2364,42 +2374,42 @@
       <c r="F6" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="21" t="s">
+      <c r="G6" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="74" t="s">
         <v>10</v>
       </c>
       <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="86"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
       <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.55" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -2408,38 +2418,38 @@
       <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G8" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="16" t="s">
+      <c r="G8" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="74" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="A9" s="76"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="22"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="75"/>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="12"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="19" t="s">
+      <c r="A10" s="76"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -2448,38 +2458,38 @@
       <c r="F10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="16" t="s">
+      <c r="G10" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="79" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="A11" s="76"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="22"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="80"/>
       <c r="I11" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="19" t="s">
+      <c r="A12" s="76"/>
+      <c r="B12" s="76"/>
+      <c r="C12" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="77" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
@@ -2488,39 +2498,39 @@
       <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="16" t="s">
+      <c r="G12" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="79" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="A13" s="76"/>
+      <c r="B13" s="76"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="18"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="80"/>
       <c r="I13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="81" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="74" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -2529,31 +2539,31 @@
       <c r="E14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="88" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="21"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="21"/>
+      <c r="G14" s="74"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="74"/>
     </row>
     <row r="15" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="22"/>
+      <c r="A15" s="85"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="24"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="22"/>
+      <c r="F15" s="89"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="75"/>
     </row>
     <row r="16" spans="1:9" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2571,8 +2581,8 @@
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="27"/>
+      <c r="A17" s="86"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2590,10 +2600,10 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="76" t="s">
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -2619,8 +2629,8 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
+      <c r="A19" s="76"/>
+      <c r="B19" s="76"/>
       <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
@@ -2632,8 +2642,8 @@
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
+      <c r="A20" s="76"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
@@ -2659,30 +2669,6 @@
   </sheetData>
   <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="38">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="G8:G9"/>
@@ -2697,6 +2683,30 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2705,6 +2715,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFE4529-F873-47C7-8ABD-E340549D4809}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2746,7 +2757,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2754,7 +2765,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>7</v>
@@ -2803,7 +2814,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>8</v>
@@ -2882,7 +2893,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>7</v>
@@ -2895,7 +2906,7 @@
       </c>
       <c r="F8" s="11"/>
       <c r="G8" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H8" s="11"/>
     </row>
@@ -2912,7 +2923,7 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2929,7 +2940,7 @@
       </c>
       <c r="F10" s="11"/>
       <c r="G10" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="11"/>
     </row>
@@ -2964,16 +2975,16 @@
         <v>11</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H12" s="11"/>
     </row>
@@ -2984,13 +2995,13 @@
         <v>12</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>10</v>

</xml_diff>